<commit_message>
volunteers prototype excel import made, and social card complex import in progress
</commit_message>
<xml_diff>
--- a/src/routes/general/volunteers.xlsx
+++ b/src/routes/general/volunteers.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="card" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="volunteers" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t xml:space="preserve">Electroingeneer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manik</t>
   </si>
 </sst>
 </file>
@@ -83,7 +80,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -125,12 +122,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -280,7 +271,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -367,24 +358,24 @@
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.3185185185185"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.4481481481482"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.437037037037"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.337037037037"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.2962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.9555555555556"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.6185185185185"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.5407407407407"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.1518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,8 +435,8 @@
       <c r="G2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>17</v>
+      <c r="H2" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>500</v>
@@ -453,9 +444,7 @@
       <c r="J2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K2" s="12" t="n">
-        <v>1</v>
-      </c>
+      <c r="K2" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>